<commit_message>
Updated sample data for Task #1094: Multiple payees
</commit_message>
<xml_diff>
--- a/SampleData/samplegen-test/TestData/FullSampleDataDefinition.xlsx
+++ b/SampleData/samplegen-test/TestData/FullSampleDataDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\SampleData\samplegen-test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7699744-EA3C-4CFA-969F-7BE7348F261D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F845ED-B557-4576-A926-A128431770EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3070" yWindow="3930" windowWidth="16440" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
+    <workbookView xWindow="650" yWindow="1970" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="95">
   <si>
     <t>Housing:Mortgage Interest</t>
   </si>
@@ -225,9 +225,6 @@
     <t>GEICO Homeowners Insurance</t>
   </si>
   <si>
-    <t>Big Megacorp</t>
-  </si>
-  <si>
     <t>Netflix</t>
   </si>
   <si>
@@ -270,15 +267,9 @@
     <t>Ralph's</t>
   </si>
   <si>
-    <t>Bed Bath &amp; Beyond</t>
-  </si>
-  <si>
     <t>Connor Construction</t>
   </si>
   <si>
-    <t>Big Plates</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -300,9 +291,6 @@
     <t>Food:Away:Coffee</t>
   </si>
   <si>
-    <t>Starbucks</t>
-  </si>
-  <si>
     <t>YearlyAmount</t>
   </si>
   <si>
@@ -316,6 +304,21 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Bed Bath &amp; Beyond,Target,Container Store</t>
+  </si>
+  <si>
+    <t>Megacorp, Inc.</t>
+  </si>
+  <si>
+    <t>Applebees,Olive Garden,Spaghetti Factory</t>
+  </si>
+  <si>
+    <t>Starbucks,Uptown Espresso,Tim Horton's</t>
+  </si>
+  <si>
+    <t>Megacorp Inc.</t>
   </si>
 </sst>
 </file>
@@ -720,7 +723,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,19 +744,19 @@
         <v>52</v>
       </c>
       <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -761,7 +764,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1">
         <f>-800*12</f>
@@ -777,7 +780,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -798,7 +801,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -869,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1">
         <f>-300*12</f>
@@ -1013,7 +1016,7 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1">
         <f>-200*12</f>
@@ -1034,7 +1037,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1">
         <f>-350*52</f>
@@ -1052,17 +1055,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1">
         <f>-52*3*7.5</f>
         <v>-1170</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
@@ -1073,17 +1076,17 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1">
         <f>-52*3*50</f>
         <v>-7800</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
@@ -1097,7 +1100,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1">
         <f>-400</f>
@@ -1118,7 +1121,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1">
         <f>-1200</f>
@@ -1139,7 +1142,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1">
         <f>-150*12</f>
@@ -1160,7 +1163,7 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1">
         <f>-40*6</f>
@@ -1181,7 +1184,7 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1">
         <f>-250</f>
@@ -1202,7 +1205,7 @@
         <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1">
         <f>-200*12</f>
@@ -1223,7 +1226,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1">
         <f>52*-35</f>
@@ -1265,7 +1268,7 @@
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="1">
         <f>-300</f>
@@ -1286,7 +1289,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1">
         <f>-400*12</f>
@@ -1307,7 +1310,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1">
         <f>-2000</f>
@@ -1328,7 +1331,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="1">
         <f>-12*12</f>
@@ -1349,7 +1352,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="1">
         <f>-15*12</f>
@@ -1370,7 +1373,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1">
         <f>-25*12</f>
@@ -1391,7 +1394,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1">
         <f>-125*4</f>
@@ -1412,13 +1415,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C33" s="1">
         <v>120000</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -1439,7 +1442,7 @@
         <v>4000</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1460,7 +1463,7 @@
         <v>-16488</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -1481,7 +1484,7 @@
         <v>-7440</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -1502,7 +1505,7 @@
         <v>-1752</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
@@ -1523,7 +1526,7 @@
         <v>-6240</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -1544,7 +1547,7 @@
         <v>-1152</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -1565,7 +1568,7 @@
         <v>-6000</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1586,7 +1589,7 @@
         <v>-4000</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -1607,7 +1610,7 @@
         <v>-19000</v>
       </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -1628,7 +1631,7 @@
         <v>-200</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -1649,7 +1652,7 @@
         <v>-50</v>
       </c>
       <c r="D44" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -1666,7 +1669,7 @@
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1">
         <v>25000</v>
@@ -1686,7 +1689,7 @@
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1">
         <f>1200</f>

</xml_diff>